<commit_message>
Reverting to the state of the project at f414f31adfa3
</commit_message>
<xml_diff>
--- a/labels.xlsx
+++ b/labels.xlsx
@@ -576,7 +576,7 @@
     <t xml:space="preserve">社会公共服务</t>
   </si>
   <si>
-    <t xml:space="preserve">dd</t>
+    <t xml:space="preserve">ff</t>
   </si>
 </sst>
 </file>
@@ -831,10 +831,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D142" activeCellId="0" sqref="D142"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H142" activeCellId="0" sqref="H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1678,7 +1678,7 @@
       <c r="A142" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D142" s="20" t="s">
+      <c r="H142" s="20" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>